<commit_message>
Versión prototipo del programa.
</commit_message>
<xml_diff>
--- a/Backend_webAPI_ASP.NETCore/wwwroot/Uploads/Lista de contactos.xlsx
+++ b/Backend_webAPI_ASP.NETCore/wwwroot/Uploads/Lista de contactos.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0272BD72-D685-4FF9-AE7C-651B1CF37AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="234">
   <si>
     <t>nombre</t>
   </si>
@@ -148,12 +149,585 @@
   </si>
   <si>
     <t>aliquam@hotmail.com</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Little</t>
+  </si>
+  <si>
+    <t>633.310.2673x35702</t>
+  </si>
+  <si>
+    <t>melissajohnston@yahoo.com</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Stafford</t>
+  </si>
+  <si>
+    <t>(423)354-7936x02827</t>
+  </si>
+  <si>
+    <t>gutierreznatalie@wallace.com</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Jimenez</t>
+  </si>
+  <si>
+    <t>841.135.6413</t>
+  </si>
+  <si>
+    <t>uwise@gmail.com</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Shannon</t>
+  </si>
+  <si>
+    <t>001-160-082-0908x138</t>
+  </si>
+  <si>
+    <t>melissajefferson@reed.com</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Mooney</t>
+  </si>
+  <si>
+    <t>186-498-5204</t>
+  </si>
+  <si>
+    <t>rachelcole@yahoo.com</t>
+  </si>
+  <si>
+    <t>Calvin</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>490-753-4909</t>
+  </si>
+  <si>
+    <t>bacosta@washington.net</t>
+  </si>
+  <si>
+    <t>Brenda</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>(195)282-9901x27762</t>
+  </si>
+  <si>
+    <t>elizabeth52@nelson.org</t>
+  </si>
+  <si>
+    <t>Erica</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>001-090-868-1352x68647</t>
+  </si>
+  <si>
+    <t>nicole25@davis.biz</t>
+  </si>
+  <si>
+    <t>Timothy</t>
+  </si>
+  <si>
+    <t>Powell</t>
+  </si>
+  <si>
+    <t>+1-316-529-7294x70100</t>
+  </si>
+  <si>
+    <t>djoyce@bailey.info</t>
+  </si>
+  <si>
+    <t>Heidi</t>
+  </si>
+  <si>
+    <t>Dorsey</t>
+  </si>
+  <si>
+    <t>720.230.9319</t>
+  </si>
+  <si>
+    <t>ochoajessica@farmer-buchanan.com</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Krause</t>
+  </si>
+  <si>
+    <t>(252)758-4783x09290</t>
+  </si>
+  <si>
+    <t>jeremy63@garrison.com</t>
+  </si>
+  <si>
+    <t>Kimberly</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>001-785-490-5066</t>
+  </si>
+  <si>
+    <t>tiffany83@kemp.com</t>
+  </si>
+  <si>
+    <t>Tracy</t>
+  </si>
+  <si>
+    <t>Snow</t>
+  </si>
+  <si>
+    <t>+1-680-034-9714x8302</t>
+  </si>
+  <si>
+    <t>cbowers@harris-ramirez.biz</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>Poole</t>
+  </si>
+  <si>
+    <t>+1-364-343-1377x16799</t>
+  </si>
+  <si>
+    <t>hrodriguez@anthony-contreras.org</t>
+  </si>
+  <si>
+    <t>Alison</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>403.986.1925</t>
+  </si>
+  <si>
+    <t>nunezvalerie@yahoo.com</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Harmon</t>
+  </si>
+  <si>
+    <t>3801111623</t>
+  </si>
+  <si>
+    <t>nhanna@reyes-gonzales.com</t>
+  </si>
+  <si>
+    <t>Anthony</t>
+  </si>
+  <si>
+    <t>Kelley</t>
+  </si>
+  <si>
+    <t>(420)756-0276</t>
+  </si>
+  <si>
+    <t>ovega@pierce.com</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>(936)224-7228x5531</t>
+  </si>
+  <si>
+    <t>edward03@hotmail.com</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Brooks</t>
+  </si>
+  <si>
+    <t>676-126-6422x9464</t>
+  </si>
+  <si>
+    <t>holly95@brown.info</t>
+  </si>
+  <si>
+    <t>Elaine</t>
+  </si>
+  <si>
+    <t>Evans</t>
+  </si>
+  <si>
+    <t>+1-309-667-8925x337</t>
+  </si>
+  <si>
+    <t>travis20@patel.org</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>001-092-076-6004</t>
+  </si>
+  <si>
+    <t>luke72@ball.info</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>Hawkins</t>
+  </si>
+  <si>
+    <t>+1-756-949-6885x43988</t>
+  </si>
+  <si>
+    <t>ronald77@gmail.com</t>
+  </si>
+  <si>
+    <t>Linda</t>
+  </si>
+  <si>
+    <t>Rogers</t>
+  </si>
+  <si>
+    <t>7324394904</t>
+  </si>
+  <si>
+    <t>kwilkinson@copeland.biz</t>
+  </si>
+  <si>
+    <t>Dana</t>
+  </si>
+  <si>
+    <t>Reed</t>
+  </si>
+  <si>
+    <t>457-623-6406</t>
+  </si>
+  <si>
+    <t>morrowdavid@barnett-hughes.com</t>
+  </si>
+  <si>
+    <t>Kelsey</t>
+  </si>
+  <si>
+    <t>Robinson</t>
+  </si>
+  <si>
+    <t>367-559-4278</t>
+  </si>
+  <si>
+    <t>mariosoto@gmail.com</t>
+  </si>
+  <si>
+    <t>Monica</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t>001-183-327-4947x58594</t>
+  </si>
+  <si>
+    <t>phillipbrown@hernandez.com</t>
+  </si>
+  <si>
+    <t>Carl</t>
+  </si>
+  <si>
+    <t>Hampton</t>
+  </si>
+  <si>
+    <t>001-143-943-3656</t>
+  </si>
+  <si>
+    <t>lopezsharon@griffith.com</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>804.882.6511</t>
+  </si>
+  <si>
+    <t>mfowler@gmail.com</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
+  </si>
+  <si>
+    <t>Sloan</t>
+  </si>
+  <si>
+    <t>0560842211</t>
+  </si>
+  <si>
+    <t>jamie18@yahoo.com</t>
+  </si>
+  <si>
+    <t>Diane</t>
+  </si>
+  <si>
+    <t>Pham</t>
+  </si>
+  <si>
+    <t>757-702-6395x1633</t>
+  </si>
+  <si>
+    <t>nnelson@hutchinson.info</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Marks</t>
+  </si>
+  <si>
+    <t>+1-779-741-8169</t>
+  </si>
+  <si>
+    <t>rubenchapman@hotmail.com</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>001-465-711-4799x99906</t>
+  </si>
+  <si>
+    <t>teresasmith@garcia.net</t>
+  </si>
+  <si>
+    <t>Samantha</t>
+  </si>
+  <si>
+    <t>6000289902</t>
+  </si>
+  <si>
+    <t>jenniferschultz@yahoo.com</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Ramos</t>
+  </si>
+  <si>
+    <t>001-759-196-5152x6574</t>
+  </si>
+  <si>
+    <t>garciamelissa@decker.biz</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Figueroa</t>
+  </si>
+  <si>
+    <t>258.683.4975x50605</t>
+  </si>
+  <si>
+    <t>angela85@hotmail.com</t>
+  </si>
+  <si>
+    <t>Spencer</t>
+  </si>
+  <si>
+    <t>945.137.2103</t>
+  </si>
+  <si>
+    <t>emily45@espinoza.com</t>
+  </si>
+  <si>
+    <t>Breanna</t>
+  </si>
+  <si>
+    <t>001-328-690-7935</t>
+  </si>
+  <si>
+    <t>cassandrajordan@cook.info</t>
+  </si>
+  <si>
+    <t>Cameron</t>
+  </si>
+  <si>
+    <t>Lewis</t>
+  </si>
+  <si>
+    <t>021-464-1200</t>
+  </si>
+  <si>
+    <t>christinajenkins@yahoo.com</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Mahoney</t>
+  </si>
+  <si>
+    <t>500.788.6430</t>
+  </si>
+  <si>
+    <t>sandralittle@gmail.com</t>
+  </si>
+  <si>
+    <t>Alexander</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>001-097-571-4354x289</t>
+  </si>
+  <si>
+    <t>bryanharris@lewis-bowman.net</t>
+  </si>
+  <si>
+    <t>Denise</t>
+  </si>
+  <si>
+    <t>(573)405-8687</t>
+  </si>
+  <si>
+    <t>misty81@beard.com</t>
+  </si>
+  <si>
+    <t>Tyler</t>
+  </si>
+  <si>
+    <t>(976)011-3966x6497</t>
+  </si>
+  <si>
+    <t>escobarjason@gmail.com</t>
+  </si>
+  <si>
+    <t>Dean</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>461.796.1954x2147</t>
+  </si>
+  <si>
+    <t>karenfigueroa@wright.info</t>
+  </si>
+  <si>
+    <t>Whitney</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>372.690.3469x952</t>
+  </si>
+  <si>
+    <t>reesekayla@gmail.com</t>
+  </si>
+  <si>
+    <t>Ricardo</t>
+  </si>
+  <si>
+    <t>Mcdonald</t>
+  </si>
+  <si>
+    <t>(384)483-9533x7663</t>
+  </si>
+  <si>
+    <t>elizabethlong@johnston.info</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>Moreno</t>
+  </si>
+  <si>
+    <t>914-939-6569x985</t>
+  </si>
+  <si>
+    <t>beth79@gmail.com</t>
+  </si>
+  <si>
+    <t>Derek</t>
+  </si>
+  <si>
+    <t>Hamilton</t>
+  </si>
+  <si>
+    <t>(714)570-0238</t>
+  </si>
+  <si>
+    <t>pagecarol@gmail.com</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>001-157-309-9272</t>
+  </si>
+  <si>
+    <t>vanessa76@yahoo.com</t>
+  </si>
+  <si>
+    <t>Padilla</t>
+  </si>
+  <si>
+    <t>1792459381</t>
+  </si>
+  <si>
+    <t>theresapowell@villegas.net</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>(348)571-8324x0570</t>
+  </si>
+  <si>
+    <t>fullerdeborah@davis.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -196,9 +770,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,19 +1053,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -504,7 +1081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -518,7 +1095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -532,7 +1109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -546,7 +1123,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -560,7 +1137,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -574,7 +1151,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -588,7 +1165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -602,7 +1179,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -616,7 +1193,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -630,7 +1207,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -642,6 +1219,706 @@
       </c>
       <c r="D11" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>